<commit_message>
finished conversion to kg
</commit_message>
<xml_diff>
--- a/project/DB/all_list_database.xlsx
+++ b/project/DB/all_list_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J254"/>
+  <dimension ref="A1:K254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>quantities</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>kg_quantities_per_portion</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -527,6 +532,9 @@
           <t>4 tbsp</t>
         </is>
       </c>
+      <c r="K2" t="n">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -575,6 +583,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K3" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -623,6 +634,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K4" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -667,6 +681,9 @@
           <t>¼ tsp</t>
         </is>
       </c>
+      <c r="K5" t="n">
+        <v>0.0002053716666666667</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -715,6 +732,9 @@
           <t>2 x 400g cans chopped</t>
         </is>
       </c>
+      <c r="K6" t="n">
+        <v>0.1333333333333333</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -763,6 +783,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K7" t="n">
+        <v>0.0008214866666666666</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -811,6 +834,9 @@
           <t>6 tbsp</t>
         </is>
       </c>
+      <c r="K8" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -859,6 +885,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K9" t="n">
+        <v>0.06666666666666667</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -907,6 +936,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K10" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -955,6 +987,9 @@
           <t>70g</t>
         </is>
       </c>
+      <c r="K11" t="n">
+        <v>0.01166666666666667</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1003,6 +1038,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K12" t="n">
+        <v>0.008333333333333333</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1047,6 +1085,9 @@
           <t>½ small bunch of</t>
         </is>
       </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1095,6 +1136,9 @@
           <t>120g</t>
         </is>
       </c>
+      <c r="K14" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1143,6 +1187,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K15" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1191,6 +1238,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K16" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1235,6 +1285,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K17" t="n">
+        <v>0.00123223</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1283,6 +1336,9 @@
           <t>80g</t>
         </is>
       </c>
+      <c r="K18" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1331,6 +1387,9 @@
           <t>600g</t>
         </is>
       </c>
+      <c r="K19" t="n">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1379,6 +1438,9 @@
           <t>400g can</t>
         </is>
       </c>
+      <c r="K20" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1427,6 +1489,9 @@
           <t>100ml</t>
         </is>
       </c>
+      <c r="K21" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1475,6 +1540,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K22" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1519,6 +1587,9 @@
         </is>
       </c>
       <c r="J23" t="inlineStr"/>
+      <c r="K23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1567,6 +1638,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K24" t="n">
+        <v>0.05000000000000001</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1615,6 +1689,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K25" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1663,6 +1740,9 @@
           <t>8 tbsp</t>
         </is>
       </c>
+      <c r="K26" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1711,6 +1791,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K27" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1759,6 +1842,9 @@
           <t>125g</t>
         </is>
       </c>
+      <c r="K28" t="n">
+        <v>0.02083333333333333</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1807,6 +1893,9 @@
           <t>handful</t>
         </is>
       </c>
+      <c r="K29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1855,6 +1944,9 @@
           <t>100g</t>
         </is>
       </c>
+      <c r="K30" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1903,6 +1995,9 @@
           <t>160g</t>
         </is>
       </c>
+      <c r="K31" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1951,6 +2046,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K32" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1999,6 +2097,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K33" t="n">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2043,6 +2144,9 @@
           <t>½ tsp</t>
         </is>
       </c>
+      <c r="K34" t="n">
+        <v>0.00123223</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2087,6 +2191,9 @@
           <t>good handful</t>
         </is>
       </c>
+      <c r="K35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2131,6 +2238,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K36" t="n">
+        <v>0.00492892</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2179,6 +2289,9 @@
           <t>few drops</t>
         </is>
       </c>
+      <c r="K37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2227,6 +2340,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K38" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2275,6 +2391,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K39" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2323,6 +2442,9 @@
           <t>280g</t>
         </is>
       </c>
+      <c r="K40" t="n">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2371,6 +2493,9 @@
           <t>1kg</t>
         </is>
       </c>
+      <c r="K41" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2419,6 +2544,9 @@
           <t>4 tbsp</t>
         </is>
       </c>
+      <c r="K42" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2467,6 +2595,9 @@
           <t>6</t>
         </is>
       </c>
+      <c r="K43" t="n">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -2507,6 +2638,9 @@
       </c>
       <c r="I44" t="inlineStr"/>
       <c r="J44" t="inlineStr"/>
+      <c r="K44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2551,6 +2685,9 @@
           <t>6 tbsp</t>
         </is>
       </c>
+      <c r="K45" t="n">
+        <v>0.0225</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -2595,6 +2732,9 @@
           <t>6 tbsp</t>
         </is>
       </c>
+      <c r="K46" t="n">
+        <v>0.0225</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -2643,6 +2783,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K47" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2691,6 +2834,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K48" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -2739,6 +2885,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K49" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -2787,6 +2936,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K50" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -2835,6 +2987,9 @@
           <t>200ml</t>
         </is>
       </c>
+      <c r="K51" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -2879,6 +3034,9 @@
           <t>½ tsp</t>
         </is>
       </c>
+      <c r="K52" t="n">
+        <v>0.00123223</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -2927,6 +3085,9 @@
           <t>100g</t>
         </is>
       </c>
+      <c r="K53" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -2975,6 +3136,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K54" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -3023,6 +3187,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K55" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -3071,6 +3238,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K56" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3119,6 +3289,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K57" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3167,6 +3340,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K58" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3211,6 +3387,9 @@
         </is>
       </c>
       <c r="J59" t="inlineStr"/>
+      <c r="K59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3255,6 +3434,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K60" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -3299,6 +3481,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K61" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3347,6 +3532,9 @@
           <t>30g</t>
         </is>
       </c>
+      <c r="K62" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3395,6 +3583,9 @@
           <t>100g</t>
         </is>
       </c>
+      <c r="K63" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3439,6 +3630,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K64" t="n">
+        <v>0.00246446</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3487,6 +3681,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K65" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3535,6 +3732,9 @@
           <t>1½ tbsp</t>
         </is>
       </c>
+      <c r="K66" t="n">
+        <v>0.005625</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3583,6 +3783,9 @@
           <t>1kg</t>
         </is>
       </c>
+      <c r="K67" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3631,6 +3834,9 @@
           <t>500g</t>
         </is>
       </c>
+      <c r="K68" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3679,6 +3885,9 @@
           <t>320g</t>
         </is>
       </c>
+      <c r="K69" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3727,6 +3936,9 @@
           <t xml:space="preserve">1½kg boneless </t>
         </is>
       </c>
+      <c r="K70" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3775,6 +3987,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K71" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3823,6 +4038,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K72" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3871,6 +4089,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K73" t="n">
+        <v>0.0025</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3915,6 +4136,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K74" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3959,6 +4183,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K75" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -4007,6 +4234,9 @@
           <t xml:space="preserve">432g can </t>
         </is>
       </c>
+      <c r="K76" t="n">
+        <v>0.07199999999999999</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -4051,6 +4281,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K77" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -4095,6 +4328,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K78" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
@@ -4139,6 +4375,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K79" t="n">
+        <v>0.0008214866666666666</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -4183,6 +4422,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K80" t="n">
+        <v>0.0008214866666666666</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -4231,6 +4473,9 @@
           <t xml:space="preserve">grating of fresh </t>
         </is>
       </c>
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -4279,6 +4524,9 @@
           <t>2½ tbsp</t>
         </is>
       </c>
+      <c r="K82" t="n">
+        <v>0.006249999999999999</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
@@ -4327,6 +4575,9 @@
           <t>1kg</t>
         </is>
       </c>
+      <c r="K83" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -4375,6 +4626,9 @@
           <t>100g</t>
         </is>
       </c>
+      <c r="K84" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
@@ -4423,6 +4677,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K85" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -4467,6 +4724,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K86" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -4515,6 +4775,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K87" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
@@ -4563,6 +4826,9 @@
           <t>3 tbsp</t>
         </is>
       </c>
+      <c r="K88" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
@@ -4611,6 +4877,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K89" t="n">
+        <v>0.0025</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -4659,6 +4928,9 @@
           <t>150ml</t>
         </is>
       </c>
+      <c r="K90" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -4703,6 +4975,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K91" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -4751,6 +5026,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K92" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -4799,6 +5077,9 @@
           <t>375g</t>
         </is>
       </c>
+      <c r="K93" t="n">
+        <v>0.0625</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -4847,6 +5128,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K94" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -4895,6 +5179,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K95" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
@@ -4943,6 +5230,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K96" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -4991,6 +5281,9 @@
           <t>400g can</t>
         </is>
       </c>
+      <c r="K97" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
@@ -5039,6 +5332,9 @@
           <t>100ml</t>
         </is>
       </c>
+      <c r="K98" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -5087,6 +5383,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K99" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -5135,6 +5434,9 @@
           <t>3 tbsp</t>
         </is>
       </c>
+      <c r="K100" t="n">
+        <v>0.0225</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
@@ -5179,6 +5481,9 @@
           <t>½ tbsp</t>
         </is>
       </c>
+      <c r="K101" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -5227,6 +5532,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K102" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
@@ -5275,6 +5583,9 @@
           <t>1½ tbsp</t>
         </is>
       </c>
+      <c r="K103" t="n">
+        <v>0.005625</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -5323,6 +5634,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K104" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -5371,6 +5685,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K105" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
@@ -5419,6 +5736,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K106" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
@@ -5463,6 +5783,9 @@
           <t>½ tsp</t>
         </is>
       </c>
+      <c r="K107" t="n">
+        <v>0.000616115</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -5511,6 +5834,9 @@
           <t>2 x 400g cans chopped</t>
         </is>
       </c>
+      <c r="K108" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -5559,6 +5885,9 @@
           <t>100g</t>
         </is>
       </c>
+      <c r="K109" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -5603,6 +5932,9 @@
           <t>500ml</t>
         </is>
       </c>
+      <c r="K110" t="n">
+        <v>0.125</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -5651,6 +5983,9 @@
           <t>12</t>
         </is>
       </c>
+      <c r="K111" t="n">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
@@ -5699,6 +6034,9 @@
           <t>150g</t>
         </is>
       </c>
+      <c r="K112" t="n">
+        <v>0.0375</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
@@ -5747,6 +6085,9 @@
           <t>½ small bunch of</t>
         </is>
       </c>
+      <c r="K113" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -5791,6 +6132,9 @@
         </is>
       </c>
       <c r="J114" t="inlineStr"/>
+      <c r="K114" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -5839,6 +6183,9 @@
           <t>400g</t>
         </is>
       </c>
+      <c r="K115" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -5887,6 +6234,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K116" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
@@ -5931,6 +6281,9 @@
           <t>½ tbsp dried</t>
         </is>
       </c>
+      <c r="K117" t="n">
+        <v>0.001875</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
@@ -5979,6 +6332,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K118" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
@@ -6023,6 +6379,9 @@
           <t>½ tsp</t>
         </is>
       </c>
+      <c r="K119" t="n">
+        <v>0.000616115</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -6067,6 +6426,9 @@
           <t>100ml</t>
         </is>
       </c>
+      <c r="K120" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -6115,6 +6477,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K121" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -6163,6 +6528,9 @@
           <t>½</t>
         </is>
       </c>
+      <c r="K122" t="n">
+        <v>0.0125</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -6211,6 +6579,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K123" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
@@ -6259,6 +6630,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K124" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -6299,6 +6673,9 @@
       </c>
       <c r="I125" t="inlineStr"/>
       <c r="J125" t="inlineStr"/>
+      <c r="K125" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -6343,6 +6720,9 @@
         </is>
       </c>
       <c r="J126" t="inlineStr"/>
+      <c r="K126" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -6391,6 +6771,9 @@
           <t>70g</t>
         </is>
       </c>
+      <c r="K127" t="n">
+        <v>0.01166666666666667</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -6439,6 +6822,9 @@
           <t>70g</t>
         </is>
       </c>
+      <c r="K128" t="n">
+        <v>0.01166666666666667</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -6487,6 +6873,9 @@
           <t>1l</t>
         </is>
       </c>
+      <c r="K129" t="n">
+        <v>0.1666666666666667</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
@@ -6531,6 +6920,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K130" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
@@ -6579,6 +6971,9 @@
           <t>80g</t>
         </is>
       </c>
+      <c r="K131" t="n">
+        <v>0.01333333333333333</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
@@ -6623,6 +7018,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K132" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -6667,6 +7065,9 @@
           <t xml:space="preserve">pinch of </t>
         </is>
       </c>
+      <c r="K133" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
@@ -6715,6 +7116,9 @@
           <t>600g</t>
         </is>
       </c>
+      <c r="K134" t="n">
+        <v>0.09999999999999999</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -6763,6 +7167,9 @@
           <t>250g</t>
         </is>
       </c>
+      <c r="K135" t="n">
+        <v>0.04166666666666666</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
@@ -6811,6 +7218,9 @@
           <t xml:space="preserve">1 whole </t>
         </is>
       </c>
+      <c r="K136" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -6859,6 +7269,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K137" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
@@ -6907,6 +7320,9 @@
           <t>12</t>
         </is>
       </c>
+      <c r="K138" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
@@ -6955,6 +7371,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K139" t="n">
+        <v>0.008333333333333333</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -7003,6 +7422,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K140" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
@@ -7051,6 +7473,9 @@
           <t>25g</t>
         </is>
       </c>
+      <c r="K141" t="n">
+        <v>0.0125</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -7099,6 +7524,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K142" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
@@ -7147,6 +7575,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K143" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -7195,6 +7626,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K144" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -7239,6 +7673,9 @@
           <t>small handful of</t>
         </is>
       </c>
+      <c r="K145" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
@@ -7287,6 +7724,9 @@
           <t>500g Maris Piper or</t>
         </is>
       </c>
+      <c r="K146" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -7335,6 +7775,9 @@
           <t>10 pitted</t>
         </is>
       </c>
+      <c r="K147" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
@@ -7383,6 +7826,9 @@
           <t>100ml chicken or</t>
         </is>
       </c>
+      <c r="K148" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
@@ -7431,6 +7877,9 @@
           <t>350g</t>
         </is>
       </c>
+      <c r="K149" t="n">
+        <v>0.08750000000000001</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
@@ -7479,6 +7928,9 @@
           <t>200ml</t>
         </is>
       </c>
+      <c r="K150" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
@@ -7527,6 +7979,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K151" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
@@ -7575,6 +8030,9 @@
           <t>400g</t>
         </is>
       </c>
+      <c r="K152" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
@@ -7623,6 +8081,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K153" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
@@ -7667,6 +8128,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K154" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
@@ -7715,6 +8179,9 @@
           <t>150ml</t>
         </is>
       </c>
+      <c r="K155" t="n">
+        <v>0.0375</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
@@ -7763,6 +8230,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K156" t="n">
+        <v>0.00123223</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
@@ -7811,6 +8281,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K157" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
@@ -7859,6 +8332,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K158" t="n">
+        <v>0.00123223</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
@@ -7907,6 +8383,9 @@
           <t>250g</t>
         </is>
       </c>
+      <c r="K159" t="n">
+        <v>0.0625</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
@@ -7955,6 +8434,9 @@
           <t>240g</t>
         </is>
       </c>
+      <c r="K160" t="n">
+        <v>0.08</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
@@ -8003,6 +8485,9 @@
           <t>knob of</t>
         </is>
       </c>
+      <c r="K161" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
@@ -8051,6 +8536,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K162" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
@@ -8099,6 +8587,9 @@
           <t>140g</t>
         </is>
       </c>
+      <c r="K163" t="n">
+        <v>0.04666666666666667</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
@@ -8147,6 +8638,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K164" t="n">
+        <v>0.06666666666666667</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
@@ -8195,6 +8689,9 @@
           <t>140g</t>
         </is>
       </c>
+      <c r="K165" t="n">
+        <v>0.04666666666666667</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
@@ -8239,6 +8736,9 @@
           <t>½</t>
         </is>
       </c>
+      <c r="K166" t="n">
+        <v>0.01666666666666667</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
@@ -8283,6 +8783,9 @@
           <t>small bunch of</t>
         </is>
       </c>
+      <c r="K167" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
@@ -8331,6 +8834,9 @@
           <t>650ml</t>
         </is>
       </c>
+      <c r="K168" t="n">
+        <v>0.1083333333333333</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
@@ -8379,6 +8885,9 @@
           <t>40g</t>
         </is>
       </c>
+      <c r="K169" t="n">
+        <v>0.006666666666666667</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
@@ -8427,6 +8936,9 @@
           <t>40g</t>
         </is>
       </c>
+      <c r="K170" t="n">
+        <v>0.006666666666666667</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
@@ -8471,6 +8983,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K171" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
@@ -8519,6 +9034,9 @@
           <t>150g</t>
         </is>
       </c>
+      <c r="K172" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
@@ -8567,6 +9085,9 @@
           <t>180g</t>
         </is>
       </c>
+      <c r="K173" t="n">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
@@ -8611,6 +9132,9 @@
           <t xml:space="preserve">handful of </t>
         </is>
       </c>
+      <c r="K174" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
@@ -8659,6 +9183,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K175" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
@@ -8707,6 +9234,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K176" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
@@ -8751,6 +9281,9 @@
         </is>
       </c>
       <c r="J177" t="inlineStr"/>
+      <c r="K177" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
@@ -8799,6 +9332,9 @@
           <t>350g</t>
         </is>
       </c>
+      <c r="K178" t="n">
+        <v>0.1166666666666667</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
@@ -8843,6 +9379,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K179" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
@@ -8887,6 +9426,9 @@
           <t>1 tsp</t>
         </is>
       </c>
+      <c r="K180" t="n">
+        <v>0.001642973333333333</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
@@ -8935,6 +9477,9 @@
           <t xml:space="preserve">1½ tbsp </t>
         </is>
       </c>
+      <c r="K181" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
@@ -8983,6 +9528,9 @@
           <t xml:space="preserve">1 large </t>
         </is>
       </c>
+      <c r="K182" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
@@ -9031,6 +9579,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K183" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
@@ -9079,6 +9630,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K184" t="n">
+        <v>0.005</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
@@ -9127,6 +9681,9 @@
           <t xml:space="preserve">2 x 400g cans chopped </t>
         </is>
       </c>
+      <c r="K185" t="n">
+        <v>0.2666666666666667</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
@@ -9175,6 +9732,9 @@
           <t>2 tsp</t>
         </is>
       </c>
+      <c r="K186" t="n">
+        <v>0.003285946666666666</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
@@ -9223,6 +9783,9 @@
           <t xml:space="preserve">150g ball </t>
         </is>
       </c>
+      <c r="K187" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
@@ -9271,6 +9834,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K188" t="n">
+        <v>0.1333333333333333</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
@@ -9319,6 +9885,9 @@
           <t>25g</t>
         </is>
       </c>
+      <c r="K189" t="n">
+        <v>0.008333333333333333</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
@@ -9363,6 +9932,9 @@
         </is>
       </c>
       <c r="J190" t="inlineStr"/>
+      <c r="K190" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
@@ -9411,6 +9983,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K191" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
@@ -9459,6 +10034,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K192" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
@@ -9503,6 +10081,9 @@
           <t>1½ tbsp</t>
         </is>
       </c>
+      <c r="K193" t="n">
+        <v>0.005625</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
@@ -9551,6 +10132,9 @@
           <t>8</t>
         </is>
       </c>
+      <c r="K194" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
@@ -9595,6 +10179,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K195" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -9643,6 +10230,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K196" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
@@ -9687,6 +10277,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K197" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
@@ -9735,6 +10328,9 @@
           <t>125g</t>
         </is>
       </c>
+      <c r="K198" t="n">
+        <v>0.03125</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
@@ -9783,6 +10379,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K199" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
@@ -9831,6 +10430,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K200" t="n">
+        <v>0.07500000000000001</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
@@ -9879,6 +10481,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K201" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
@@ -9927,6 +10532,9 @@
           <t>700g</t>
         </is>
       </c>
+      <c r="K202" t="n">
+        <v>0.2333333333333334</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
@@ -9975,6 +10583,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K203" t="n">
+        <v>0.01</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
@@ -10023,6 +10634,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K204" t="n">
+        <v>0.03333333333333333</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -10071,6 +10685,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K205" t="n">
+        <v>0.1333333333333333</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
@@ -10115,6 +10732,9 @@
           <t xml:space="preserve">small bunch of </t>
         </is>
       </c>
+      <c r="K206" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
@@ -10159,6 +10779,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K207" t="n">
+        <v>0.1333333333333333</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
@@ -10203,6 +10826,9 @@
         </is>
       </c>
       <c r="J208" t="inlineStr"/>
+      <c r="K208" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
@@ -10247,6 +10873,9 @@
           <t xml:space="preserve">½ tsp </t>
         </is>
       </c>
+      <c r="K209" t="n">
+        <v>0.0008214866666666666</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -10295,6 +10924,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K210" t="n">
+        <v>0.09999999999999999</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
@@ -10343,6 +10975,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K211" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
@@ -10391,6 +11026,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K212" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
@@ -10435,6 +11073,9 @@
           <t>3 tbsp</t>
         </is>
       </c>
+      <c r="K213" t="n">
+        <v>0.0225</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
@@ -10483,6 +11124,9 @@
           <t xml:space="preserve">400g can </t>
         </is>
       </c>
+      <c r="K214" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
@@ -10531,6 +11175,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K215" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
@@ -10579,6 +11226,9 @@
           <t xml:space="preserve">1 large or 2 small </t>
         </is>
       </c>
+      <c r="K216" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
@@ -10623,6 +11273,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K217" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
@@ -10667,6 +11320,9 @@
         </is>
       </c>
       <c r="J218" t="inlineStr"/>
+      <c r="K218" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
@@ -10715,6 +11371,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K219" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
@@ -10759,6 +11418,9 @@
           <t>1 thumb-sized piece</t>
         </is>
       </c>
+      <c r="K220" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
@@ -10807,6 +11469,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K221" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
@@ -10855,6 +11520,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K222" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
@@ -10899,6 +11567,9 @@
           <t>2-3 tbsp</t>
         </is>
       </c>
+      <c r="K223" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
@@ -10947,6 +11618,9 @@
           <t>400g can chopped</t>
         </is>
       </c>
+      <c r="K224" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
@@ -10995,6 +11669,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K225" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
@@ -11043,6 +11720,9 @@
           <t>½ tbsp</t>
         </is>
       </c>
+      <c r="K226" t="n">
+        <v>0.001875</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
@@ -11087,6 +11767,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K227" t="n">
+        <v>0.07500000000000001</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
@@ -11135,6 +11818,9 @@
           <t>200g</t>
         </is>
       </c>
+      <c r="K228" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
@@ -11183,6 +11869,9 @@
           <t>3 tbsp</t>
         </is>
       </c>
+      <c r="K229" t="n">
+        <v>0.01125</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
@@ -11231,6 +11920,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K230" t="n">
+        <v>0.075</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
@@ -11279,6 +11971,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K231" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
@@ -11323,6 +12018,9 @@
           <t>½ bunch of</t>
         </is>
       </c>
+      <c r="K232" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
@@ -11367,6 +12065,9 @@
         </is>
       </c>
       <c r="J233" t="inlineStr"/>
+      <c r="K233" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -11415,6 +12116,9 @@
           <t>2</t>
         </is>
       </c>
+      <c r="K234" t="n">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -11463,6 +12167,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K235" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
@@ -11507,6 +12214,9 @@
           <t>4 tbsp</t>
         </is>
       </c>
+      <c r="K236" t="n">
+        <v>0.015</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
@@ -11551,6 +12261,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K237" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
@@ -11599,6 +12312,9 @@
           <t>3</t>
         </is>
       </c>
+      <c r="K238" t="n">
+        <v>0.07500000000000001</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
@@ -11647,6 +12363,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K239" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
@@ -11691,6 +12410,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K240" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
@@ -11739,6 +12461,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K241" t="n">
+        <v>0.075</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
@@ -11787,6 +12512,9 @@
           <t>50ml</t>
         </is>
       </c>
+      <c r="K242" t="n">
+        <v>0.0125</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
@@ -11831,6 +12559,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K243" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
@@ -11879,6 +12610,9 @@
           <t>4</t>
         </is>
       </c>
+      <c r="K244" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
@@ -11927,6 +12661,9 @@
           <t>1</t>
         </is>
       </c>
+      <c r="K245" t="n">
+        <v>0.025</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
@@ -11975,6 +12712,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K246" t="n">
+        <v>0.075</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
@@ -12023,6 +12763,9 @@
           <t>300g</t>
         </is>
       </c>
+      <c r="K247" t="n">
+        <v>0.075</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
@@ -12071,6 +12814,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K248" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
@@ -12119,6 +12865,9 @@
           <t>1 large bunch of</t>
         </is>
       </c>
+      <c r="K249" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
@@ -12167,6 +12916,9 @@
           <t>1 large</t>
         </is>
       </c>
+      <c r="K250" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
@@ -12215,6 +12967,9 @@
           <t>2 tbsp</t>
         </is>
       </c>
+      <c r="K251" t="n">
+        <v>0.0075</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
@@ -12263,6 +13018,9 @@
           <t>1 tbsp</t>
         </is>
       </c>
+      <c r="K252" t="n">
+        <v>0.00375</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -12311,6 +13069,9 @@
           <t>50g</t>
         </is>
       </c>
+      <c r="K253" t="n">
+        <v>0.0125</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
@@ -12358,6 +13119,9 @@
         <is>
           <t>200g</t>
         </is>
+      </c>
+      <c r="K254" t="n">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>